<commit_message>
Related Accounts was modified by GIT
</commit_message>
<xml_diff>
--- a/b2130-MyAccount-RelatedAccounts/Main.rvl.xlsx
+++ b/b2130-MyAccount-RelatedAccounts/Main.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>Flow</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>2000</t>
+  </si>
+  <si>
+    <t>500</t>
   </si>
 </sst>
 </file>
@@ -527,7 +530,7 @@
         <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -569,7 +572,7 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">

</xml_diff>